<commit_message>
port to feather esp32 v2
</commit_message>
<xml_diff>
--- a/hardware/Pinouts.xlsx
+++ b/hardware/Pinouts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylej\dev\plastic-scanner\v1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devos\Nextcloud\Projects\Plastic Scanner 2024\plastic-scanner-kyle\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA37135-B2E4-434F-8416-377726A2A692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6578A33-C8BF-4CD9-962E-09DD92FDD5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="9300" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>PIN</t>
   </si>
@@ -112,6 +112,21 @@
   </si>
   <si>
     <t>SCL/22</t>
+  </si>
+  <si>
+    <t>feather esp32 v2</t>
+  </si>
+  <si>
+    <t>rst</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>output?</t>
+  </si>
+  <si>
+    <t>buzzer</t>
   </si>
 </sst>
 </file>
@@ -208,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -222,6 +237,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,15 +521,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H15"/>
+  <dimension ref="B1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>9</v>
       </c>
@@ -525,7 +543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" ht="33" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -544,8 +562,11 @@
       <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -565,7 +586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
@@ -585,7 +606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -604,8 +625,11 @@
       <c r="H5" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
@@ -624,8 +648,11 @@
       <c r="H6" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -644,8 +671,11 @@
       <c r="H7" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
@@ -658,8 +688,11 @@
       <c r="H8" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
@@ -672,8 +705,11 @@
       <c r="H9" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
@@ -686,8 +722,11 @@
       <c r="H10" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
@@ -700,8 +739,11 @@
       <c r="H11" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
@@ -714,8 +756,11 @@
       <c r="H12" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
@@ -728,8 +773,11 @@
       <c r="H13" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
         <v>23</v>
       </c>
@@ -742,8 +790,11 @@
       <c r="H14" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
@@ -755,6 +806,31 @@
       </c>
       <c r="H15" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="I15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="E17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17">
+        <v>17</v>
+      </c>
+      <c r="I17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="6">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>